<commit_message>
Add Simulations & Carnaught maps
</commit_message>
<xml_diff>
--- a/Exercise_1/writing/FSM_States.xlsx
+++ b/Exercise_1/writing/FSM_States.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\HW2-Exercise\Exercise_1\writing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\HW2-Project\Exercise_1\writing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DD59519-F679-4958-85B6-5A1DE432F759}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{727B35C7-D8C4-4303-B2ED-8F1D839FE087}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{C29D9B36-9969-44FD-AEE6-6D81136DF297}"/>
+    <workbookView xWindow="20970" yWindow="7440" windowWidth="27750" windowHeight="14685" xr2:uid="{C29D9B36-9969-44FD-AEE6-6D81136DF297}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -296,6 +296,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -303,15 +312,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -489,10 +489,10 @@
     <tableColumn id="9" xr3:uid="{9C472BB6-2335-4891-85DD-288AABB2FE9E}" name="_D2" dataDxfId="3">
       <calculatedColumnFormula>(1-Table1[[#This Row],[D2]])*(1-Table1[[#This Row],[D1]])*Table1[[#This Row],[X]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{D5BAF824-589C-445D-9334-4A585BEE3142}" name="_D1" dataDxfId="1">
+    <tableColumn id="10" xr3:uid="{D5BAF824-589C-445D-9334-4A585BEE3142}" name="_D1" dataDxfId="2">
       <calculatedColumnFormula>Table1[[#This Row],[D2]]+(1-Table1[[#This Row],[X]])*(1-Table1[[#This Row],[D0]])+Table1[[#This Row],[X]]*Table1[[#This Row],[D0]]*Table1[[#This Row],[D1]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{1438480F-8621-4AA0-953D-877544125639}" name="_D0" dataDxfId="2">
+    <tableColumn id="11" xr3:uid="{1438480F-8621-4AA0-953D-877544125639}" name="_D0" dataDxfId="1">
       <calculatedColumnFormula>Table1[[#This Row],[X]]*Table1[[#This Row],[D2]]+(1-Table1[[#This Row],[X]])*(1-Table1[[#This Row],[D2]])*(1-(Table1[[#This Row],[D1]]*(1-Table1[[#This Row],[D0]])))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="12" xr3:uid="{1426278F-A330-4DDF-8F9B-02363C142E80}" name="_Y" dataDxfId="0">
@@ -802,8 +802,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33CB1BC2-C430-4FAD-B89D-4CDFA87C1CFF}">
   <dimension ref="B1:M12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="185" zoomScaleNormal="280" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -817,19 +817,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="12"/>
-      <c r="D1" s="13"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="16"/>
       <c r="E1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="12"/>
-      <c r="H1" s="13"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="16"/>
       <c r="I1" s="6" t="s">
         <v>11</v>
       </c>
@@ -901,15 +901,15 @@
         <f>(1-Table1[[#This Row],[D2]])*(1-Table1[[#This Row],[D1]])*Table1[[#This Row],[X]]</f>
         <v>0</v>
       </c>
-      <c r="K3" s="14">
+      <c r="K3" s="11">
         <f>Table1[[#This Row],[D2]]+(1-Table1[[#This Row],[X]])*(1-Table1[[#This Row],[D0]])+Table1[[#This Row],[X]]*Table1[[#This Row],[D0]]*Table1[[#This Row],[D1]]</f>
         <v>1</v>
       </c>
-      <c r="L3" s="14">
+      <c r="L3" s="11">
         <f>Table1[[#This Row],[X]]*Table1[[#This Row],[D2]]+(1-Table1[[#This Row],[X]])*(1-Table1[[#This Row],[D2]])*(1-(Table1[[#This Row],[D1]]*(1-Table1[[#This Row],[D0]])))</f>
         <v>1</v>
       </c>
-      <c r="M3" s="15">
+      <c r="M3" s="12">
         <f>(1-Table1[[#This Row],[D0'']])*Table1[[#This Row],[X]]</f>
         <v>0</v>
       </c>
@@ -939,7 +939,7 @@
       <c r="I4" s="2">
         <v>1</v>
       </c>
-      <c r="J4" s="14">
+      <c r="J4" s="11">
         <f>(1-Table1[[#This Row],[D2]])*(1-Table1[[#This Row],[D1]])*Table1[[#This Row],[X]]</f>
         <v>1</v>
       </c>
@@ -951,7 +951,7 @@
         <f>Table1[[#This Row],[X]]*Table1[[#This Row],[D2]]+(1-Table1[[#This Row],[X]])*(1-Table1[[#This Row],[D2]])*(1-(Table1[[#This Row],[D1]]*(1-Table1[[#This Row],[D0]])))</f>
         <v>0</v>
       </c>
-      <c r="M4" s="16">
+      <c r="M4" s="13">
         <f>(1-Table1[[#This Row],[D0'']])*Table1[[#This Row],[X]]</f>
         <v>1</v>
       </c>
@@ -989,11 +989,11 @@
         <f>Table1[[#This Row],[D2]]+(1-Table1[[#This Row],[X]])*(1-Table1[[#This Row],[D0]])+Table1[[#This Row],[X]]*Table1[[#This Row],[D0]]*Table1[[#This Row],[D1]]</f>
         <v>0</v>
       </c>
-      <c r="L5" s="14">
+      <c r="L5" s="11">
         <f>Table1[[#This Row],[X]]*Table1[[#This Row],[D2]]+(1-Table1[[#This Row],[X]])*(1-Table1[[#This Row],[D2]])*(1-(Table1[[#This Row],[D1]]*(1-Table1[[#This Row],[D0]])))</f>
         <v>1</v>
       </c>
-      <c r="M5" s="15">
+      <c r="M5" s="12">
         <f>(1-Table1[[#This Row],[D0'']])*Table1[[#This Row],[X]]</f>
         <v>0</v>
       </c>
@@ -1023,7 +1023,7 @@
       <c r="I6" s="2">
         <v>1</v>
       </c>
-      <c r="J6" s="14">
+      <c r="J6" s="11">
         <f>(1-Table1[[#This Row],[D2]])*(1-Table1[[#This Row],[D1]])*Table1[[#This Row],[X]]</f>
         <v>1</v>
       </c>
@@ -1035,7 +1035,7 @@
         <f>Table1[[#This Row],[X]]*Table1[[#This Row],[D2]]+(1-Table1[[#This Row],[X]])*(1-Table1[[#This Row],[D2]])*(1-(Table1[[#This Row],[D1]]*(1-Table1[[#This Row],[D0]])))</f>
         <v>0</v>
       </c>
-      <c r="M6" s="16">
+      <c r="M6" s="13">
         <f>(1-Table1[[#This Row],[D0'']])*Table1[[#This Row],[X]]</f>
         <v>1</v>
       </c>
@@ -1069,7 +1069,7 @@
         <f>(1-Table1[[#This Row],[D2]])*(1-Table1[[#This Row],[D1]])*Table1[[#This Row],[X]]</f>
         <v>0</v>
       </c>
-      <c r="K7" s="14">
+      <c r="K7" s="11">
         <f>Table1[[#This Row],[D2]]+(1-Table1[[#This Row],[X]])*(1-Table1[[#This Row],[D0]])+Table1[[#This Row],[X]]*Table1[[#This Row],[D0]]*Table1[[#This Row],[D1]]</f>
         <v>1</v>
       </c>
@@ -1077,7 +1077,7 @@
         <f>Table1[[#This Row],[X]]*Table1[[#This Row],[D2]]+(1-Table1[[#This Row],[X]])*(1-Table1[[#This Row],[D2]])*(1-(Table1[[#This Row],[D1]]*(1-Table1[[#This Row],[D0]])))</f>
         <v>0</v>
       </c>
-      <c r="M7" s="15">
+      <c r="M7" s="12">
         <f>(1-Table1[[#This Row],[D0'']])*Table1[[#This Row],[X]]</f>
         <v>0</v>
       </c>
@@ -1119,7 +1119,7 @@
         <f>Table1[[#This Row],[X]]*Table1[[#This Row],[D2]]+(1-Table1[[#This Row],[X]])*(1-Table1[[#This Row],[D2]])*(1-(Table1[[#This Row],[D1]]*(1-Table1[[#This Row],[D0]])))</f>
         <v>0</v>
       </c>
-      <c r="M8" s="16">
+      <c r="M8" s="13">
         <f>(1-Table1[[#This Row],[D0'']])*Table1[[#This Row],[X]]</f>
         <v>1</v>
       </c>
@@ -1157,11 +1157,11 @@
         <f>Table1[[#This Row],[D2]]+(1-Table1[[#This Row],[X]])*(1-Table1[[#This Row],[D0]])+Table1[[#This Row],[X]]*Table1[[#This Row],[D0]]*Table1[[#This Row],[D1]]</f>
         <v>0</v>
       </c>
-      <c r="L9" s="14">
+      <c r="L9" s="11">
         <f>Table1[[#This Row],[X]]*Table1[[#This Row],[D2]]+(1-Table1[[#This Row],[X]])*(1-Table1[[#This Row],[D2]])*(1-(Table1[[#This Row],[D1]]*(1-Table1[[#This Row],[D0]])))</f>
         <v>1</v>
       </c>
-      <c r="M9" s="15">
+      <c r="M9" s="12">
         <f>(1-Table1[[#This Row],[D0'']])*Table1[[#This Row],[X]]</f>
         <v>0</v>
       </c>
@@ -1195,7 +1195,7 @@
         <f>(1-Table1[[#This Row],[D2]])*(1-Table1[[#This Row],[D1]])*Table1[[#This Row],[X]]</f>
         <v>0</v>
       </c>
-      <c r="K10" s="14">
+      <c r="K10" s="11">
         <f>Table1[[#This Row],[D2]]+(1-Table1[[#This Row],[X]])*(1-Table1[[#This Row],[D0]])+Table1[[#This Row],[X]]*Table1[[#This Row],[D0]]*Table1[[#This Row],[D1]]</f>
         <v>1</v>
       </c>
@@ -1203,7 +1203,7 @@
         <f>Table1[[#This Row],[X]]*Table1[[#This Row],[D2]]+(1-Table1[[#This Row],[X]])*(1-Table1[[#This Row],[D2]])*(1-(Table1[[#This Row],[D1]]*(1-Table1[[#This Row],[D0]])))</f>
         <v>0</v>
       </c>
-      <c r="M10" s="16">
+      <c r="M10" s="13">
         <f>(1-Table1[[#This Row],[D0'']])*Table1[[#This Row],[X]]</f>
         <v>1</v>
       </c>
@@ -1237,7 +1237,7 @@
         <f>(1-Table1[[#This Row],[D2]])*(1-Table1[[#This Row],[D1]])*Table1[[#This Row],[X]]</f>
         <v>0</v>
       </c>
-      <c r="K11" s="14">
+      <c r="K11" s="11">
         <f>Table1[[#This Row],[D2]]+(1-Table1[[#This Row],[X]])*(1-Table1[[#This Row],[D0]])+Table1[[#This Row],[X]]*Table1[[#This Row],[D0]]*Table1[[#This Row],[D1]]</f>
         <v>2</v>
       </c>
@@ -1245,7 +1245,7 @@
         <f>Table1[[#This Row],[X]]*Table1[[#This Row],[D2]]+(1-Table1[[#This Row],[X]])*(1-Table1[[#This Row],[D2]])*(1-(Table1[[#This Row],[D1]]*(1-Table1[[#This Row],[D0]])))</f>
         <v>0</v>
       </c>
-      <c r="M11" s="15">
+      <c r="M11" s="12">
         <f>(1-Table1[[#This Row],[D0'']])*Table1[[#This Row],[X]]</f>
         <v>0</v>
       </c>
@@ -1279,15 +1279,15 @@
         <f>(1-Table1[[#This Row],[D2]])*(1-Table1[[#This Row],[D1]])*Table1[[#This Row],[X]]</f>
         <v>0</v>
       </c>
-      <c r="K12" s="14">
+      <c r="K12" s="11">
         <f>Table1[[#This Row],[D2]]+(1-Table1[[#This Row],[X]])*(1-Table1[[#This Row],[D0]])+Table1[[#This Row],[X]]*Table1[[#This Row],[D0]]*Table1[[#This Row],[D1]]</f>
         <v>1</v>
       </c>
-      <c r="L12" s="14">
+      <c r="L12" s="11">
         <f>Table1[[#This Row],[X]]*Table1[[#This Row],[D2]]+(1-Table1[[#This Row],[X]])*(1-Table1[[#This Row],[D2]])*(1-(Table1[[#This Row],[D1]]*(1-Table1[[#This Row],[D0]])))</f>
         <v>1</v>
       </c>
-      <c r="M12" s="15">
+      <c r="M12" s="12">
         <f>(1-Table1[[#This Row],[D0'']])*Table1[[#This Row],[X]]</f>
         <v>0</v>
       </c>

</xml_diff>